<commit_message>
Nov 30 update support card crawler, set Ramonu unique effect id to 16
</commit_message>
<xml_diff>
--- a/Document/支援卡固有.xlsx
+++ b/Document/支援卡固有.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
   <si>
     <t>原始固有</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -439,10 +439,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>每个速度技能+4%训练，共5层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>高峰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -468,6 +464,18 @@
   </si>
   <si>
     <t>DD，光钻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个加速度技能+X，共3层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>力高峰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个X技能+Y，共Z层</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,7 +483,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +500,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -616,18 +641,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -919,7 +944,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1025,10 +1050,10 @@
       <c r="M3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="P3" s="18"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1061,8 +1086,8 @@
       <c r="M4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1092,8 +1117,8 @@
       <c r="M5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1105,16 +1130,16 @@
       <c r="C6" s="12">
         <v>103</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="16" t="s">
         <v>77</v>
       </c>
       <c r="L6" s="1">
@@ -1123,10 +1148,10 @@
       <c r="N6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="P6" s="18"/>
+      <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1156,8 +1181,8 @@
       <c r="N7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1187,8 +1212,8 @@
       <c r="N8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
     </row>
     <row r="9" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1221,8 +1246,8 @@
       <c r="N9" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1261,8 +1286,8 @@
       <c r="N10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
     </row>
     <row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1301,8 +1326,8 @@
       <c r="N11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
     </row>
     <row r="12" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1332,8 +1357,8 @@
       <c r="N12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
     </row>
     <row r="13" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1363,8 +1388,8 @@
       <c r="N13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
     </row>
     <row r="14" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1394,8 +1419,8 @@
       <c r="N14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
     </row>
     <row r="15" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1422,8 +1447,8 @@
       <c r="N15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
     </row>
     <row r="16" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1453,8 +1478,8 @@
       <c r="N16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
     </row>
     <row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1487,8 +1512,8 @@
       <c r="N17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
     </row>
     <row r="18" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1518,8 +1543,8 @@
       <c r="N18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
     </row>
     <row r="19" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1553,13 +1578,13 @@
         <v>16</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1592,8 +1617,8 @@
       <c r="N20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
     </row>
     <row r="21" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1623,8 +1648,8 @@
       <c r="N21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
     </row>
     <row r="22" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1633,17 +1658,17 @@
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L22" s="18">
         <v>19</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="M22" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="N22" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
     </row>
     <row r="23" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1652,17 +1677,17 @@
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="19">
         <v>20</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="N23" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
     </row>
     <row r="24" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1671,17 +1696,17 @@
       <c r="B24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L24" s="19">
+      <c r="L24" s="16">
         <v>21</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="N24" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="N24" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
     </row>
     <row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1690,7 +1715,15 @@
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="16"/>
+      <c r="L25" s="18">
+        <v>22</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="26" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">

</xml_diff>

<commit_message>
Feb 24 UAF version, update Larc data
</commit_message>
<xml_diff>
--- a/Document/支援卡固有.xlsx
+++ b/Document/支援卡固有.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>原始固有</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -443,39 +443,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>每个速度技能+X，共3层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>跳舞城，根黑楼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个回体技能+X，共3层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>速善信，耐桂冠</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DD类</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DD，光钻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个加速度技能+X，共3层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>力高峰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>每个X技能+Y，共Z层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羁绊&gt;80时根据卡组增加副属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巨匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羁绊&gt;60时，支援卡咕率下降</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>凉花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>凉花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预留</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巨匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巨匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DD，光钻，万籁</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -512,11 +520,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -596,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,10 +654,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -943,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1050,10 +1061,10 @@
       <c r="M3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="P3" s="17"/>
+      <c r="P3" s="18"/>
     </row>
     <row r="4" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1086,8 +1097,8 @@
       <c r="M4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1117,8 +1128,8 @@
       <c r="M5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
     </row>
     <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1148,10 +1159,10 @@
       <c r="N6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="P6" s="17"/>
+      <c r="P6" s="18"/>
     </row>
     <row r="7" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1181,8 +1192,8 @@
       <c r="N7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
     </row>
     <row r="8" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1212,8 +1223,8 @@
       <c r="N8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
     </row>
     <row r="9" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1246,8 +1257,8 @@
       <c r="N9" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
     </row>
     <row r="10" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1286,8 +1297,8 @@
       <c r="N10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1326,8 +1337,8 @@
       <c r="N11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
     </row>
     <row r="12" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1357,8 +1368,8 @@
       <c r="N12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
     </row>
     <row r="13" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1388,8 +1399,8 @@
       <c r="N13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
     </row>
     <row r="14" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1419,8 +1430,8 @@
       <c r="N14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
     </row>
     <row r="15" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1447,8 +1458,8 @@
       <c r="N15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
     </row>
     <row r="16" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1478,8 +1489,8 @@
       <c r="N16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
     </row>
     <row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1512,8 +1523,8 @@
       <c r="N17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
     </row>
     <row r="18" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1543,8 +1554,8 @@
       <c r="N18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
     </row>
     <row r="19" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1578,13 +1589,13 @@
         <v>16</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1617,8 +1628,8 @@
       <c r="N20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
     </row>
     <row r="21" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1648,8 +1659,8 @@
       <c r="N21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
     </row>
     <row r="22" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1658,14 +1669,30 @@
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="18">
+      <c r="C22" s="3">
+        <v>119</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="1">
+        <v>50</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>60</v>
+      </c>
+      <c r="L22" s="19">
         <v>19</v>
       </c>
-      <c r="M22" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="N22" s="19" t="s">
-        <v>107</v>
+      <c r="M22" s="19"/>
+      <c r="N22" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
@@ -1677,14 +1704,35 @@
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="19">
+      <c r="C23" s="3">
+        <v>120</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>80</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2</v>
+      </c>
+      <c r="L23" s="20">
         <v>20</v>
       </c>
-      <c r="M23" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="N23" s="19" t="s">
-        <v>109</v>
+      <c r="M23" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="N23" s="20" t="s">
+        <v>115</v>
       </c>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
@@ -1700,10 +1748,10 @@
         <v>21</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N24" s="16" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
@@ -1715,15 +1763,13 @@
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="19">
         <v>22</v>
       </c>
-      <c r="M25" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="N25" s="19" t="s">
+      <c r="M25" s="19" t="s">
         <v>113</v>
       </c>
+      <c r="N25" s="17"/>
     </row>
     <row r="26" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">

</xml_diff>